<commit_message>
update tc mobile - auth
</commit_message>
<xml_diff>
--- a/data-test/WEB_Register.xlsx
+++ b/data-test/WEB_Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFDE7FB-D0F9-42D6-9659-5FEBDB581B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E97330-D4EB-4F9E-87A4-F83C37844A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="3465" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
+    <workbookView xWindow="4950" yWindow="3315" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,10 @@
     <t>salsabila1@gmail.com</t>
   </si>
   <si>
-    <t>1234sals!s</t>
-  </si>
-  <si>
-    <t>sals1234@gmail.com</t>
+    <t>emailsalsaaaa@gmail.com</t>
+  </si>
+  <si>
+    <t>emailsalsa2</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Testing Web - 13/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Register.xlsx
+++ b/data-test/WEB_Register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E97330-D4EB-4F9E-87A4-F83C37844A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE753C0E-4AFA-40C5-AFD3-BD7346F4BF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4950" yWindow="3315" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
   </bookViews>
@@ -71,10 +71,10 @@
     <t>salsabila1@gmail.com</t>
   </si>
   <si>
-    <t>emailsalsaaaa@gmail.com</t>
-  </si>
-  <si>
-    <t>emailsalsa2</t>
+    <t>halosalsa</t>
+  </si>
+  <si>
+    <t>halosalsa@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Test Suite Mobile Auth - 14/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Register.xlsx
+++ b/data-test/WEB_Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58231FF5-2F9E-4CAF-834D-890B34FB264B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8117DB5-4095-4F8A-B0B8-6BD8F94FBE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,10 @@
     <t>salsabila1@gmail.com</t>
   </si>
   <si>
-    <t>halosalsa3</t>
-  </si>
-  <si>
-    <t>halosalsa3@gmail.com</t>
+    <t>halosalsa4</t>
+  </si>
+  <si>
+    <t>halosalsa4@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Test Suite Web - 15/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Register.xlsx
+++ b/data-test/WEB_Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8117DB5-4095-4F8A-B0B8-6BD8F94FBE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10FA25-4264-44B0-8F8E-BF46175D53E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,10 @@
     <t>salsabila1@gmail.com</t>
   </si>
   <si>
-    <t>halosalsa4</t>
-  </si>
-  <si>
-    <t>halosalsa4@gmail.com</t>
+    <t>halosalsa5</t>
+  </si>
+  <si>
+    <t>halosalsa5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Testing Web - 17/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Register.xlsx
+++ b/data-test/WEB_Register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10FA25-4264-44B0-8F8E-BF46175D53E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5B8B18-3CB5-4A54-9DB1-55AF77FCD96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9270" xr2:uid="{51919866-AF37-4B83-B7BB-E4652AF2DB38}"/>
   </bookViews>
@@ -71,10 +71,10 @@
     <t>salsabila1@gmail.com</t>
   </si>
   <si>
-    <t>halosalsa5</t>
-  </si>
-  <si>
-    <t>halosalsa5@gmail.com</t>
+    <t>halosalsa37</t>
+  </si>
+  <si>
+    <t>halosalsa37@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{B2619720-32D7-4BF9-B345-53088CF3A682}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{9ACCDBE4-379C-4AFB-B70E-646CDA102ED9}"/>
-    <hyperlink ref="B7" r:id="rId3" display="bila@123" xr:uid="{6129EF02-824C-4458-BCD0-96874FFAEF39}"/>
+    <hyperlink ref="B7" r:id="rId3" display="halosalsa27@gmail.com" xr:uid="{6129EF02-824C-4458-BCD0-96874FFAEF39}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{108D5743-EF9C-41B3-99C5-209B14E13F8E}"/>
     <hyperlink ref="B8" r:id="rId5" xr:uid="{EB1DC34C-E0DD-4DBE-B582-D1144331B9BB}"/>
   </hyperlinks>

</xml_diff>